<commit_message>
chore(data): update war reports with fresh data (GMT-3)
</commit_message>
<xml_diff>
--- a/data/relatorio_participacao_guerra.xlsx
+++ b/data/relatorio_participacao_guerra.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="75">
   <si>
     <t>Nome</t>
   </si>
@@ -43,178 +43,199 @@
     <t>JOSA</t>
   </si>
   <si>
+    <t>nova</t>
+  </si>
+  <si>
+    <t>Yzzy the best ¿</t>
+  </si>
+  <si>
+    <t>Gustavo</t>
+  </si>
+  <si>
+    <t>sj pro</t>
+  </si>
+  <si>
+    <t>alm ícaro⁷⁷⁷</t>
+  </si>
+  <si>
+    <t>- ROJÎ</t>
+  </si>
+  <si>
+    <t>Alvaro</t>
+  </si>
+  <si>
+    <t>Sotto ツ</t>
+  </si>
+  <si>
+    <t>Felipe</t>
+  </si>
+  <si>
+    <t>Zenitsu愛</t>
+  </si>
+  <si>
+    <t>danilo</t>
+  </si>
+  <si>
+    <t>PedrinhoR14</t>
+  </si>
+  <si>
+    <t>Dockz</t>
+  </si>
+  <si>
+    <t>5C4RF4C3</t>
+  </si>
+  <si>
+    <t>luba</t>
+  </si>
+  <si>
+    <t>ed</t>
+  </si>
+  <si>
+    <t>caioba_</t>
+  </si>
+  <si>
+    <t>BRS⚔️ASHURA</t>
+  </si>
+  <si>
+    <t>john</t>
+  </si>
+  <si>
+    <t>Theus Carvalho</t>
+  </si>
+  <si>
+    <t>mini.peka</t>
+  </si>
+  <si>
+    <t>kauansin777</t>
+  </si>
+  <si>
+    <t>Luiz Fernando™</t>
+  </si>
+  <si>
+    <t>dogmal</t>
+  </si>
+  <si>
+    <t>Rodolfos</t>
+  </si>
+  <si>
+    <t>polaris</t>
+  </si>
+  <si>
+    <t>Chetto</t>
+  </si>
+  <si>
+    <t>Teixeirazzqw</t>
+  </si>
+  <si>
+    <t>WILLIAN</t>
+  </si>
+  <si>
+    <t>Mila</t>
+  </si>
+  <si>
+    <t>RaiNascimento</t>
+  </si>
+  <si>
+    <t>tavin</t>
+  </si>
+  <si>
+    <t>^_^^_^</t>
+  </si>
+  <si>
+    <t>Bruno</t>
+  </si>
+  <si>
+    <t>⭐O SENTINELA ⭐</t>
+  </si>
+  <si>
+    <t>domador de but</t>
+  </si>
+  <si>
+    <t>filho de duque</t>
+  </si>
+  <si>
+    <t>O GUARDIÃO</t>
+  </si>
+  <si>
+    <t>luck</t>
+  </si>
+  <si>
+    <t>Nico</t>
+  </si>
+  <si>
+    <t>Pedro PH</t>
+  </si>
+  <si>
+    <t>DGJ-DAVI</t>
+  </si>
+  <si>
+    <t>Luciano</t>
+  </si>
+  <si>
+    <t>Daniele❤</t>
+  </si>
+  <si>
+    <t>GabiMalvadeza</t>
+  </si>
+  <si>
+    <t>super</t>
+  </si>
+  <si>
+    <t>EDDIE</t>
+  </si>
+  <si>
+    <t>WvCly</t>
+  </si>
+  <si>
+    <t>nivelador</t>
+  </si>
+  <si>
+    <t>andrebts</t>
+  </si>
+  <si>
+    <t>OneDePrata</t>
+  </si>
+  <si>
+    <t>isp</t>
+  </si>
+  <si>
+    <t>gabiggoughost</t>
+  </si>
+  <si>
+    <t>Grimmer 狼</t>
+  </si>
+  <si>
     <t>joão3:16</t>
   </si>
   <si>
-    <t>nova</t>
-  </si>
-  <si>
-    <t>Chetto</t>
-  </si>
-  <si>
-    <t>Yzzy the best ¿</t>
-  </si>
-  <si>
-    <t>Mila</t>
-  </si>
-  <si>
-    <t>sj pro</t>
-  </si>
-  <si>
-    <t>Nico</t>
-  </si>
-  <si>
-    <t>RaiNascimento</t>
-  </si>
-  <si>
     <t>RobaFrag</t>
   </si>
   <si>
-    <t>Luciano</t>
-  </si>
-  <si>
-    <t>alm ícaro⁷⁷⁷</t>
-  </si>
-  <si>
-    <t>Daniele❤</t>
-  </si>
-  <si>
-    <t>Alvaro</t>
-  </si>
-  <si>
-    <t>Teixeirazzqw</t>
-  </si>
-  <si>
-    <t>tavin</t>
-  </si>
-  <si>
     <t>51 é pinga</t>
   </si>
   <si>
-    <t>Sotto ツ</t>
-  </si>
-  <si>
-    <t>super</t>
-  </si>
-  <si>
-    <t>EDDIE</t>
-  </si>
-  <si>
     <t>gabriel 3$</t>
   </si>
   <si>
-    <t>^_^^_^</t>
-  </si>
-  <si>
-    <t>Bruno</t>
-  </si>
-  <si>
-    <t>Zenitsu愛</t>
-  </si>
-  <si>
-    <t>⭐O SENTINELA ⭐</t>
-  </si>
-  <si>
-    <t>domador de but</t>
-  </si>
-  <si>
-    <t>danilo</t>
-  </si>
-  <si>
-    <t>WvCly</t>
-  </si>
-  <si>
-    <t>PedrinhoR14</t>
-  </si>
-  <si>
-    <t>Dockz</t>
-  </si>
-  <si>
-    <t>isp</t>
-  </si>
-  <si>
-    <t>5C4RF4C3</t>
-  </si>
-  <si>
     <t>Asten Acady</t>
   </si>
   <si>
-    <t>Pedro PH</t>
-  </si>
-  <si>
-    <t>DGJ-DAVI</t>
-  </si>
-  <si>
-    <t>luba</t>
-  </si>
-  <si>
-    <t>nivelador</t>
-  </si>
-  <si>
-    <t>gabiggoughost</t>
-  </si>
-  <si>
-    <t>ed</t>
-  </si>
-  <si>
     <t>ZackThunder</t>
   </si>
   <si>
-    <t>caioba_</t>
-  </si>
-  <si>
-    <t>O GUARDIÃO</t>
-  </si>
-  <si>
-    <t>Grimmer 狼</t>
-  </si>
-  <si>
-    <t>BRS⚔️ASHURA</t>
-  </si>
-  <si>
-    <t>andrebts</t>
-  </si>
-  <si>
-    <t>john</t>
-  </si>
-  <si>
-    <t>OneDePrata</t>
-  </si>
-  <si>
-    <t>luck</t>
-  </si>
-  <si>
-    <t>Theus Carvalho</t>
-  </si>
-  <si>
-    <t>polaris</t>
-  </si>
-  <si>
-    <t>mini.peka</t>
-  </si>
-  <si>
     <t>mathi❄️</t>
   </si>
   <si>
-    <t>Rodolfos</t>
-  </si>
-  <si>
-    <t>kauansin777</t>
-  </si>
-  <si>
     <t>Gustavo Clash</t>
   </si>
   <si>
-    <t>Luiz Fernando™</t>
-  </si>
-  <si>
     <t>Razoável</t>
   </si>
   <si>
+    <t>Verificar</t>
+  </si>
+  <si>
     <t>Ok</t>
-  </si>
-  <si>
-    <t>Verificar</t>
   </si>
   <si>
     <t>Guerra Atual</t>
@@ -575,7 +596,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H57"/>
+  <dimension ref="A1:H64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -612,10 +633,10 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="C2" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="D2">
         <v>12</v>
@@ -638,25 +659,25 @@
         <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="C3" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="D3">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="E3">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="F3">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="G3">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="H3">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -664,10 +685,10 @@
         <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="C4" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -690,25 +711,25 @@
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="C5" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="D5">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="E5">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="F5">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="G5">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="H5">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -716,19 +737,19 @@
         <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="C6" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="D6">
         <v>0</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -742,25 +763,25 @@
         <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="C7" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="D7">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="E7">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="F7">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="G7">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="H7">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -768,19 +789,19 @@
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="C8" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="D8">
         <v>0</v>
       </c>
       <c r="E8">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="F8">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G8">
         <v>0</v>
@@ -794,25 +815,25 @@
         <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="C9" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="D9">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E9">
         <v>14</v>
       </c>
       <c r="F9">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="G9">
         <v>14</v>
       </c>
       <c r="H9">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -820,25 +841,25 @@
         <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="C10" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="F10">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="G10">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="H10">
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -846,25 +867,25 @@
         <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="C11" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="D11">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="E11">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="F11">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="G11">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="H11">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -872,25 +893,25 @@
         <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="C12" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="D12">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="E12">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="F12">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G12">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H12">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -898,22 +919,22 @@
         <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="C13" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="D13">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E13">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="F13">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="G13">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H13">
         <v>0</v>
@@ -924,13 +945,13 @@
         <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="C14" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="D14">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E14">
         <v>16</v>
@@ -950,25 +971,25 @@
         <v>21</v>
       </c>
       <c r="B15" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="C15" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="D15">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E15">
         <v>14</v>
       </c>
       <c r="F15">
+        <v>16</v>
+      </c>
+      <c r="G15">
+        <v>16</v>
+      </c>
+      <c r="H15">
         <v>15</v>
-      </c>
-      <c r="G15">
-        <v>14</v>
-      </c>
-      <c r="H15">
-        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -976,13 +997,13 @@
         <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="C16" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="D16">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E16">
         <v>0</v>
@@ -1002,22 +1023,22 @@
         <v>23</v>
       </c>
       <c r="B17" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="C17" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="D17">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="E17">
+        <v>12</v>
+      </c>
+      <c r="F17">
         <v>8</v>
       </c>
-      <c r="F17">
-        <v>14</v>
-      </c>
       <c r="G17">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="H17">
         <v>16</v>
@@ -1028,10 +1049,10 @@
         <v>24</v>
       </c>
       <c r="B18" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="C18" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="D18">
         <v>16</v>
@@ -1054,25 +1075,25 @@
         <v>25</v>
       </c>
       <c r="B19" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="C19" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="D19">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="E19">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="F19">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="G19">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="H19">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -1080,13 +1101,13 @@
         <v>26</v>
       </c>
       <c r="B20" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="C20" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="D20">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E20">
         <v>16</v>
@@ -1098,7 +1119,7 @@
         <v>16</v>
       </c>
       <c r="H20">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -1106,25 +1127,25 @@
         <v>27</v>
       </c>
       <c r="B21" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="C21" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="D21">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="E21">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F21">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="G21">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="H21">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -1132,25 +1153,25 @@
         <v>28</v>
       </c>
       <c r="B22" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="C22" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="D22">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E22">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="F22">
         <v>16</v>
       </c>
       <c r="G22">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="H22">
-        <v>4</v>
+        <v>16</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -1158,25 +1179,25 @@
         <v>29</v>
       </c>
       <c r="B23" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="C23" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="D23">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="E23">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="F23">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="G23">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="H23">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -1184,25 +1205,25 @@
         <v>30</v>
       </c>
       <c r="B24" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="C24" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="D24">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="E24">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F24">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="G24">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="H24">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -1210,25 +1231,25 @@
         <v>31</v>
       </c>
       <c r="B25" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="C25" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="D25">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E25">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="F25">
         <v>12</v>
       </c>
       <c r="G25">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H25">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -1236,25 +1257,25 @@
         <v>32</v>
       </c>
       <c r="B26" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="C26" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="D26">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="E26">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="F26">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="G26">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="H26">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -1262,10 +1283,10 @@
         <v>33</v>
       </c>
       <c r="B27" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="C27" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="D27">
         <v>16</v>
@@ -1274,10 +1295,10 @@
         <v>16</v>
       </c>
       <c r="F27">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="G27">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="H27">
         <v>12</v>
@@ -1288,10 +1309,10 @@
         <v>34</v>
       </c>
       <c r="B28" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="C28" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="D28">
         <v>16</v>
@@ -1303,10 +1324,10 @@
         <v>16</v>
       </c>
       <c r="G28">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="H28">
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -1314,25 +1335,25 @@
         <v>35</v>
       </c>
       <c r="B29" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="C29" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="D29">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E29">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F29">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="G29">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="H29">
-        <v>6</v>
+        <v>15</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -1340,25 +1361,25 @@
         <v>36</v>
       </c>
       <c r="B30" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="C30" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="D30">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E30">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="F30">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="G30">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="H30">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -1366,25 +1387,25 @@
         <v>37</v>
       </c>
       <c r="B31" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="C31" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="D31">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="E31">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="F31">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="G31">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="H31">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -1392,13 +1413,13 @@
         <v>38</v>
       </c>
       <c r="B32" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="C32" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="D32">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E32">
         <v>16</v>
@@ -1418,10 +1439,10 @@
         <v>39</v>
       </c>
       <c r="B33" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="C33" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="D33">
         <v>0</v>
@@ -1444,22 +1465,22 @@
         <v>40</v>
       </c>
       <c r="B34" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="C34" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="D34">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E34">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="F34">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G34">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H34">
         <v>16</v>
@@ -1470,25 +1491,25 @@
         <v>41</v>
       </c>
       <c r="B35" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="C35" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="D35">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E35">
         <v>16</v>
       </c>
       <c r="F35">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="G35">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="H35">
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -1496,10 +1517,10 @@
         <v>42</v>
       </c>
       <c r="B36" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="C36" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="D36">
         <v>16</v>
@@ -1508,10 +1529,10 @@
         <v>16</v>
       </c>
       <c r="F36">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="G36">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="H36">
         <v>16</v>
@@ -1522,19 +1543,19 @@
         <v>43</v>
       </c>
       <c r="B37" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="C37" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="D37">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E37">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="F37">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="G37">
         <v>16</v>
@@ -1548,25 +1569,25 @@
         <v>44</v>
       </c>
       <c r="B38" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="C38" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="D38">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E38">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="F38">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="G38">
         <v>12</v>
       </c>
       <c r="H38">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -1574,25 +1595,25 @@
         <v>45</v>
       </c>
       <c r="B39" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="C39" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="D39">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="E39">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="F39">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="G39">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="H39">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:8">
@@ -1600,10 +1621,10 @@
         <v>46</v>
       </c>
       <c r="B40" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="C40" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="D40">
         <v>16</v>
@@ -1626,25 +1647,25 @@
         <v>47</v>
       </c>
       <c r="B41" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="C41" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="D41">
         <v>16</v>
       </c>
       <c r="E41">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="F41">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G41">
         <v>16</v>
       </c>
       <c r="H41">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="42" spans="1:8">
@@ -1652,25 +1673,25 @@
         <v>48</v>
       </c>
       <c r="B42" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="C42" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="D42">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="E42">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F42">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="G42">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="H42">
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="43" spans="1:8">
@@ -1678,10 +1699,10 @@
         <v>49</v>
       </c>
       <c r="B43" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="C43" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="D43">
         <v>16</v>
@@ -1690,13 +1711,13 @@
         <v>16</v>
       </c>
       <c r="F43">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="G43">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="H43">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:8">
@@ -1704,25 +1725,25 @@
         <v>50</v>
       </c>
       <c r="B44" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="C44" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="D44">
         <v>16</v>
       </c>
       <c r="E44">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="F44">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="G44">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="H44">
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="45" spans="1:8">
@@ -1730,25 +1751,25 @@
         <v>51</v>
       </c>
       <c r="B45" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="C45" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="D45">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="E45">
         <v>16</v>
       </c>
       <c r="F45">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G45">
         <v>16</v>
       </c>
       <c r="H45">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="46" spans="1:8">
@@ -1756,13 +1777,13 @@
         <v>52</v>
       </c>
       <c r="B46" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="C46" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="D46">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E46">
         <v>16</v>
@@ -1782,25 +1803,25 @@
         <v>53</v>
       </c>
       <c r="B47" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="C47" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="D47">
         <v>0</v>
       </c>
       <c r="E47">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="F47">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="G47">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="H47">
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:8">
@@ -1808,22 +1829,22 @@
         <v>54</v>
       </c>
       <c r="B48" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="C48" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="D48">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E48">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="F48">
         <v>16</v>
       </c>
       <c r="G48">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H48">
         <v>16</v>
@@ -1834,10 +1855,10 @@
         <v>55</v>
       </c>
       <c r="B49" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="C49" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="D49">
         <v>16</v>
@@ -1846,13 +1867,13 @@
         <v>16</v>
       </c>
       <c r="F49">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="G49">
         <v>16</v>
       </c>
       <c r="H49">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="50" spans="1:8">
@@ -1860,25 +1881,25 @@
         <v>56</v>
       </c>
       <c r="B50" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="C50" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="D50">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E50">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F50">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="G50">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="H50">
-        <v>16</v>
+        <v>6</v>
       </c>
     </row>
     <row r="51" spans="1:8">
@@ -1886,25 +1907,25 @@
         <v>57</v>
       </c>
       <c r="B51" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="C51" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="D51">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E51">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F51">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G51">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H51">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:8">
@@ -1912,25 +1933,25 @@
         <v>58</v>
       </c>
       <c r="B52" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="C52" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="D52">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="E52">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="F52">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="G52">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="H52">
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="53" spans="1:8">
@@ -1938,22 +1959,22 @@
         <v>59</v>
       </c>
       <c r="B53" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="C53" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="D53">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E53">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F53">
         <v>16</v>
       </c>
       <c r="G53">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H53">
         <v>16</v>
@@ -1964,10 +1985,10 @@
         <v>60</v>
       </c>
       <c r="B54" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="C54" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="D54">
         <v>16</v>
@@ -1979,10 +2000,10 @@
         <v>16</v>
       </c>
       <c r="G54">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H54">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="55" spans="1:8">
@@ -1990,25 +2011,25 @@
         <v>61</v>
       </c>
       <c r="B55" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="C55" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="D55">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E55">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F55">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="G55">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="H55">
-        <v>9</v>
+        <v>16</v>
       </c>
     </row>
     <row r="56" spans="1:8">
@@ -2016,25 +2037,25 @@
         <v>62</v>
       </c>
       <c r="B56" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="C56" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="D56">
         <v>16</v>
       </c>
       <c r="E56">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="F56">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="G56">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="H56">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:8">
@@ -2042,25 +2063,207 @@
         <v>63</v>
       </c>
       <c r="B57" t="s">
+        <v>73</v>
+      </c>
+      <c r="C57" t="s">
+        <v>74</v>
+      </c>
+      <c r="D57">
+        <v>16</v>
+      </c>
+      <c r="E57">
+        <v>16</v>
+      </c>
+      <c r="F57">
+        <v>16</v>
+      </c>
+      <c r="G57">
+        <v>16</v>
+      </c>
+      <c r="H57">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8">
+      <c r="A58" t="s">
+        <v>64</v>
+      </c>
+      <c r="B58" t="s">
+        <v>73</v>
+      </c>
+      <c r="C58" t="s">
+        <v>74</v>
+      </c>
+      <c r="D58">
+        <v>16</v>
+      </c>
+      <c r="E58">
+        <v>16</v>
+      </c>
+      <c r="F58">
+        <v>16</v>
+      </c>
+      <c r="G58">
+        <v>16</v>
+      </c>
+      <c r="H58">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8">
+      <c r="A59" t="s">
+        <v>65</v>
+      </c>
+      <c r="B59" t="s">
+        <v>73</v>
+      </c>
+      <c r="C59" t="s">
+        <v>74</v>
+      </c>
+      <c r="D59">
+        <v>16</v>
+      </c>
+      <c r="E59">
+        <v>16</v>
+      </c>
+      <c r="F59">
+        <v>16</v>
+      </c>
+      <c r="G59">
+        <v>16</v>
+      </c>
+      <c r="H59">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8">
+      <c r="A60" t="s">
         <v>66</v>
       </c>
-      <c r="C57" t="s">
+      <c r="B60" t="s">
+        <v>73</v>
+      </c>
+      <c r="C60" t="s">
+        <v>74</v>
+      </c>
+      <c r="D60">
+        <v>16</v>
+      </c>
+      <c r="E60">
+        <v>16</v>
+      </c>
+      <c r="F60">
+        <v>16</v>
+      </c>
+      <c r="G60">
+        <v>16</v>
+      </c>
+      <c r="H60">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8">
+      <c r="A61" t="s">
         <v>67</v>
       </c>
-      <c r="D57">
+      <c r="B61" t="s">
+        <v>73</v>
+      </c>
+      <c r="C61" t="s">
+        <v>74</v>
+      </c>
+      <c r="D61">
+        <v>16</v>
+      </c>
+      <c r="E61">
+        <v>16</v>
+      </c>
+      <c r="F61">
+        <v>16</v>
+      </c>
+      <c r="G61">
+        <v>16</v>
+      </c>
+      <c r="H61">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8">
+      <c r="A62" t="s">
+        <v>68</v>
+      </c>
+      <c r="B62" t="s">
+        <v>73</v>
+      </c>
+      <c r="C62" t="s">
+        <v>74</v>
+      </c>
+      <c r="D62">
+        <v>16</v>
+      </c>
+      <c r="E62">
         <v>8</v>
       </c>
-      <c r="E57">
-        <v>16</v>
-      </c>
-      <c r="F57">
-        <v>12</v>
-      </c>
-      <c r="G57">
-        <v>13</v>
-      </c>
-      <c r="H57">
+      <c r="F62">
+        <v>16</v>
+      </c>
+      <c r="G62">
+        <v>16</v>
+      </c>
+      <c r="H62">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8">
+      <c r="A63" t="s">
+        <v>69</v>
+      </c>
+      <c r="B63" t="s">
+        <v>71</v>
+      </c>
+      <c r="C63" t="s">
+        <v>74</v>
+      </c>
+      <c r="D63">
+        <v>14</v>
+      </c>
+      <c r="E63">
         <v>10</v>
+      </c>
+      <c r="F63">
+        <v>16</v>
+      </c>
+      <c r="G63">
+        <v>16</v>
+      </c>
+      <c r="H63">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8">
+      <c r="A64" t="s">
+        <v>70</v>
+      </c>
+      <c r="B64" t="s">
+        <v>73</v>
+      </c>
+      <c r="C64" t="s">
+        <v>74</v>
+      </c>
+      <c r="D64">
+        <v>16</v>
+      </c>
+      <c r="E64">
+        <v>16</v>
+      </c>
+      <c r="F64">
+        <v>16</v>
+      </c>
+      <c r="G64">
+        <v>16</v>
+      </c>
+      <c r="H64">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chore: Update dashboard data Friday 16/01
</commit_message>
<xml_diff>
--- a/data/relatorio_participacao_guerra.xlsx
+++ b/data/relatorio_participacao_guerra.xlsx
@@ -61,172 +61,172 @@
     <t>- ROJÎ</t>
   </si>
   <si>
+    <t>Felipe</t>
+  </si>
+  <si>
+    <t>Zenitsu愛</t>
+  </si>
+  <si>
+    <t>danilo</t>
+  </si>
+  <si>
+    <t>PedrinhoR14</t>
+  </si>
+  <si>
+    <t>5C4RF4C3</t>
+  </si>
+  <si>
+    <t>luba</t>
+  </si>
+  <si>
+    <t>ed</t>
+  </si>
+  <si>
+    <t>caioba_</t>
+  </si>
+  <si>
+    <t>BRS⚔️ASHURA</t>
+  </si>
+  <si>
+    <t>john</t>
+  </si>
+  <si>
+    <t>Theus Carvalho</t>
+  </si>
+  <si>
+    <t>mini.peka</t>
+  </si>
+  <si>
+    <t>kauansin777</t>
+  </si>
+  <si>
+    <t>Luiz Fernando™</t>
+  </si>
+  <si>
+    <t>dogmal</t>
+  </si>
+  <si>
+    <t>RaiNascimento</t>
+  </si>
+  <si>
+    <t>^_^^_^</t>
+  </si>
+  <si>
+    <t>Bruno</t>
+  </si>
+  <si>
+    <t>domador de but</t>
+  </si>
+  <si>
+    <t>Nico</t>
+  </si>
+  <si>
+    <t>Pedro PH</t>
+  </si>
+  <si>
+    <t>WILLIAN</t>
+  </si>
+  <si>
+    <t>gabiggoughost</t>
+  </si>
+  <si>
+    <t>polaris</t>
+  </si>
+  <si>
+    <t>Sotto ツ</t>
+  </si>
+  <si>
+    <t>mathi❄️</t>
+  </si>
+  <si>
+    <t>Gustavo Clash</t>
+  </si>
+  <si>
+    <t>Chetto</t>
+  </si>
+  <si>
+    <t>GabiMalvadeza</t>
+  </si>
+  <si>
     <t>Alvaro</t>
   </si>
   <si>
-    <t>Sotto ツ</t>
-  </si>
-  <si>
-    <t>Felipe</t>
-  </si>
-  <si>
-    <t>Zenitsu愛</t>
-  </si>
-  <si>
-    <t>danilo</t>
-  </si>
-  <si>
-    <t>PedrinhoR14</t>
+    <t>Teixeirazzqw</t>
+  </si>
+  <si>
+    <t>Rodolfos</t>
+  </si>
+  <si>
+    <t>filho de duque</t>
+  </si>
+  <si>
+    <t>luck</t>
+  </si>
+  <si>
+    <t>tavin</t>
+  </si>
+  <si>
+    <t>O GUARDIÃO</t>
+  </si>
+  <si>
+    <t>Grimmer 狼</t>
+  </si>
+  <si>
+    <t>super</t>
+  </si>
+  <si>
+    <t>EDDIE</t>
+  </si>
+  <si>
+    <t>⭐O SENTINELA ⭐</t>
+  </si>
+  <si>
+    <t>andrebts</t>
+  </si>
+  <si>
+    <t>OneDePrata</t>
   </si>
   <si>
     <t>Dockz</t>
   </si>
   <si>
-    <t>5C4RF4C3</t>
-  </si>
-  <si>
-    <t>luba</t>
-  </si>
-  <si>
-    <t>ed</t>
-  </si>
-  <si>
-    <t>caioba_</t>
-  </si>
-  <si>
-    <t>BRS⚔️ASHURA</t>
-  </si>
-  <si>
-    <t>john</t>
-  </si>
-  <si>
-    <t>Theus Carvalho</t>
-  </si>
-  <si>
-    <t>mini.peka</t>
-  </si>
-  <si>
-    <t>kauansin777</t>
-  </si>
-  <si>
-    <t>Luiz Fernando™</t>
-  </si>
-  <si>
-    <t>dogmal</t>
-  </si>
-  <si>
-    <t>Rodolfos</t>
-  </si>
-  <si>
-    <t>polaris</t>
-  </si>
-  <si>
-    <t>Chetto</t>
-  </si>
-  <si>
-    <t>Teixeirazzqw</t>
-  </si>
-  <si>
-    <t>WILLIAN</t>
-  </si>
-  <si>
     <t>Mila</t>
   </si>
   <si>
-    <t>RaiNascimento</t>
-  </si>
-  <si>
-    <t>tavin</t>
-  </si>
-  <si>
-    <t>^_^^_^</t>
-  </si>
-  <si>
-    <t>Bruno</t>
-  </si>
-  <si>
-    <t>⭐O SENTINELA ⭐</t>
-  </si>
-  <si>
-    <t>domador de but</t>
-  </si>
-  <si>
-    <t>filho de duque</t>
-  </si>
-  <si>
-    <t>O GUARDIÃO</t>
-  </si>
-  <si>
-    <t>luck</t>
-  </si>
-  <si>
-    <t>Nico</t>
-  </si>
-  <si>
-    <t>Pedro PH</t>
+    <t>RobaFrag</t>
+  </si>
+  <si>
+    <t>Daniele❤</t>
+  </si>
+  <si>
+    <t>51 é pinga</t>
+  </si>
+  <si>
+    <t>WvCly</t>
   </si>
   <si>
     <t>DGJ-DAVI</t>
   </si>
   <si>
+    <t>isp</t>
+  </si>
+  <si>
+    <t>nivelador</t>
+  </si>
+  <si>
     <t>Luciano</t>
   </si>
   <si>
-    <t>Daniele❤</t>
-  </si>
-  <si>
-    <t>GabiMalvadeza</t>
-  </si>
-  <si>
-    <t>super</t>
-  </si>
-  <si>
-    <t>EDDIE</t>
-  </si>
-  <si>
-    <t>WvCly</t>
-  </si>
-  <si>
-    <t>nivelador</t>
-  </si>
-  <si>
-    <t>andrebts</t>
-  </si>
-  <si>
-    <t>OneDePrata</t>
-  </si>
-  <si>
-    <t>isp</t>
-  </si>
-  <si>
-    <t>gabiggoughost</t>
-  </si>
-  <si>
-    <t>Grimmer 狼</t>
+    <t>gabriel 3$</t>
+  </si>
+  <si>
+    <t>ZackThunder</t>
   </si>
   <si>
     <t>joão3:16</t>
   </si>
   <si>
-    <t>RobaFrag</t>
-  </si>
-  <si>
-    <t>51 é pinga</t>
-  </si>
-  <si>
-    <t>gabriel 3$</t>
-  </si>
-  <si>
     <t>Asten Acady</t>
-  </si>
-  <si>
-    <t>ZackThunder</t>
-  </si>
-  <si>
-    <t>mathi❄️</t>
-  </si>
-  <si>
-    <t>Gustavo Clash</t>
   </si>
   <si>
     <t>Razoável</t>
@@ -815,25 +815,25 @@
         <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C9" t="s">
         <v>74</v>
       </c>
       <c r="D9">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="E9">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="F9">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="G9">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="H9">
-        <v>14</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -841,25 +841,25 @@
         <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C10" t="s">
         <v>74</v>
       </c>
       <c r="D10">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="E10">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="F10">
         <v>12</v>
       </c>
       <c r="G10">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H10">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -867,22 +867,22 @@
         <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C11" t="s">
         <v>74</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="F11">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="G11">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H11">
         <v>0</v>
@@ -893,25 +893,25 @@
         <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C12" t="s">
         <v>74</v>
       </c>
       <c r="D12">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="E12">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="F12">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="G12">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="H12">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -919,22 +919,22 @@
         <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C13" t="s">
         <v>74</v>
       </c>
       <c r="D13">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="E13">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="F13">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="G13">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H13">
         <v>0</v>
@@ -945,19 +945,19 @@
         <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C14" t="s">
         <v>74</v>
       </c>
       <c r="D14">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="E14">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F14">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="G14">
         <v>16</v>
@@ -980,7 +980,7 @@
         <v>16</v>
       </c>
       <c r="E15">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F15">
         <v>16</v>
@@ -989,7 +989,7 @@
         <v>16</v>
       </c>
       <c r="H15">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -1006,7 +1006,7 @@
         <v>0</v>
       </c>
       <c r="E16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F16">
         <v>0</v>
@@ -1029,19 +1029,19 @@
         <v>74</v>
       </c>
       <c r="D17">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E17">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="F17">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="G17">
         <v>16</v>
       </c>
       <c r="H17">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -1049,25 +1049,25 @@
         <v>24</v>
       </c>
       <c r="B18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C18" t="s">
         <v>74</v>
       </c>
       <c r="D18">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="E18">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F18">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="G18">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="H18">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -1075,25 +1075,25 @@
         <v>25</v>
       </c>
       <c r="B19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C19" t="s">
         <v>74</v>
       </c>
       <c r="D19">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="E19">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F19">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="G19">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="H19">
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -1107,19 +1107,19 @@
         <v>74</v>
       </c>
       <c r="D20">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E20">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="F20">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="G20">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="H20">
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -1136,16 +1136,16 @@
         <v>0</v>
       </c>
       <c r="E21">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F21">
+        <v>12</v>
+      </c>
+      <c r="G21">
+        <v>12</v>
+      </c>
+      <c r="H21">
         <v>9</v>
-      </c>
-      <c r="G21">
-        <v>11</v>
-      </c>
-      <c r="H21">
-        <v>12</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -1153,25 +1153,25 @@
         <v>28</v>
       </c>
       <c r="B22" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C22" t="s">
         <v>74</v>
       </c>
       <c r="D22">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E22">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="F22">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G22">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H22">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -1185,7 +1185,7 @@
         <v>74</v>
       </c>
       <c r="D23">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E23">
         <v>0</v>
@@ -1214,16 +1214,16 @@
         <v>0</v>
       </c>
       <c r="E24">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="F24">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="G24">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="H24">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -1231,13 +1231,13 @@
         <v>31</v>
       </c>
       <c r="B25" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C25" t="s">
         <v>74</v>
       </c>
       <c r="D25">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E25">
         <v>16</v>
@@ -1246,10 +1246,10 @@
         <v>12</v>
       </c>
       <c r="G25">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H25">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -1257,16 +1257,16 @@
         <v>32</v>
       </c>
       <c r="B26" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C26" t="s">
         <v>74</v>
       </c>
       <c r="D26">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E26">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="F26">
         <v>0</v>
@@ -1275,7 +1275,7 @@
         <v>0</v>
       </c>
       <c r="H26">
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -1295,10 +1295,10 @@
         <v>16</v>
       </c>
       <c r="F27">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="G27">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="H27">
         <v>12</v>
@@ -1309,22 +1309,22 @@
         <v>34</v>
       </c>
       <c r="B28" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C28" t="s">
         <v>74</v>
       </c>
       <c r="D28">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E28">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F28">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="G28">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="H28">
         <v>16</v>
@@ -1335,25 +1335,25 @@
         <v>35</v>
       </c>
       <c r="B29" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C29" t="s">
         <v>74</v>
       </c>
       <c r="D29">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E29">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="F29">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G29">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="H29">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -1367,7 +1367,7 @@
         <v>74</v>
       </c>
       <c r="D30">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E30">
         <v>0</v>
@@ -1387,25 +1387,25 @@
         <v>37</v>
       </c>
       <c r="B31" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C31" t="s">
         <v>74</v>
       </c>
       <c r="D31">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E31">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="F31">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="G31">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="H31">
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -1413,13 +1413,13 @@
         <v>38</v>
       </c>
       <c r="B32" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C32" t="s">
         <v>74</v>
       </c>
       <c r="D32">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E32">
         <v>16</v>
@@ -1439,25 +1439,25 @@
         <v>39</v>
       </c>
       <c r="B33" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C33" t="s">
         <v>74</v>
       </c>
       <c r="D33">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="E33">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="F33">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="G33">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="H33">
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -1471,16 +1471,16 @@
         <v>74</v>
       </c>
       <c r="D34">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E34">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F34">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G34">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="H34">
         <v>16</v>
@@ -1491,22 +1491,22 @@
         <v>41</v>
       </c>
       <c r="B35" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C35" t="s">
         <v>74</v>
       </c>
       <c r="D35">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E35">
         <v>16</v>
       </c>
       <c r="F35">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="G35">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="H35">
         <v>16</v>
@@ -1517,25 +1517,25 @@
         <v>42</v>
       </c>
       <c r="B36" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C36" t="s">
         <v>74</v>
       </c>
       <c r="D36">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E36">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F36">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="G36">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="H36">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -1543,25 +1543,25 @@
         <v>43</v>
       </c>
       <c r="B37" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C37" t="s">
         <v>74</v>
       </c>
       <c r="D37">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="E37">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="F37">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="G37">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="H37">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:8">
@@ -1569,25 +1569,25 @@
         <v>44</v>
       </c>
       <c r="B38" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C38" t="s">
         <v>74</v>
       </c>
       <c r="D38">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E38">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F38">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="G38">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H38">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -1601,7 +1601,7 @@
         <v>74</v>
       </c>
       <c r="D39">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E39">
         <v>0</v>
@@ -1636,10 +1636,10 @@
         <v>16</v>
       </c>
       <c r="G40">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H40">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="41" spans="1:8">
@@ -1647,25 +1647,25 @@
         <v>47</v>
       </c>
       <c r="B41" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C41" t="s">
         <v>74</v>
       </c>
       <c r="D41">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="E41">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="F41">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="G41">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="H41">
-        <v>13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:8">
@@ -1673,25 +1673,25 @@
         <v>48</v>
       </c>
       <c r="B42" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C42" t="s">
         <v>74</v>
       </c>
       <c r="D42">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E42">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F42">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="G42">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H42">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="43" spans="1:8">
@@ -1699,25 +1699,25 @@
         <v>49</v>
       </c>
       <c r="B43" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C43" t="s">
         <v>74</v>
       </c>
       <c r="D43">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E43">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="F43">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="G43">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="H43">
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="44" spans="1:8">
@@ -1737,10 +1737,10 @@
         <v>16</v>
       </c>
       <c r="F44">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="G44">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H44">
         <v>16</v>
@@ -1760,16 +1760,16 @@
         <v>16</v>
       </c>
       <c r="E45">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="F45">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="G45">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="H45">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:8">
@@ -1803,25 +1803,25 @@
         <v>53</v>
       </c>
       <c r="B47" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C47" t="s">
         <v>74</v>
       </c>
       <c r="D47">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E47">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="F47">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="G47">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="H47">
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="48" spans="1:8">
@@ -1855,13 +1855,13 @@
         <v>55</v>
       </c>
       <c r="B49" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C49" t="s">
         <v>74</v>
       </c>
       <c r="D49">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E49">
         <v>16</v>
@@ -1881,25 +1881,25 @@
         <v>56</v>
       </c>
       <c r="B50" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C50" t="s">
         <v>74</v>
       </c>
       <c r="D50">
+        <v>15</v>
+      </c>
+      <c r="E50">
         <v>8</v>
       </c>
-      <c r="E50">
-        <v>14</v>
-      </c>
       <c r="F50">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="G50">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="H50">
-        <v>6</v>
+        <v>16</v>
       </c>
     </row>
     <row r="51" spans="1:8">
@@ -1907,25 +1907,25 @@
         <v>57</v>
       </c>
       <c r="B51" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C51" t="s">
         <v>74</v>
       </c>
       <c r="D51">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E51">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="F51">
+        <v>16</v>
+      </c>
+      <c r="G51">
+        <v>16</v>
+      </c>
+      <c r="H51">
         <v>15</v>
-      </c>
-      <c r="G51">
-        <v>12</v>
-      </c>
-      <c r="H51">
-        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:8">
@@ -1933,13 +1933,13 @@
         <v>58</v>
       </c>
       <c r="B52" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C52" t="s">
         <v>74</v>
       </c>
       <c r="D52">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="E52">
         <v>16</v>
@@ -1959,22 +1959,22 @@
         <v>59</v>
       </c>
       <c r="B53" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C53" t="s">
         <v>74</v>
       </c>
       <c r="D53">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E53">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="F53">
         <v>16</v>
       </c>
       <c r="G53">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H53">
         <v>16</v>
@@ -2020,7 +2020,7 @@
         <v>16</v>
       </c>
       <c r="E55">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F55">
         <v>16</v>
@@ -2037,25 +2037,25 @@
         <v>62</v>
       </c>
       <c r="B56" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C56" t="s">
         <v>74</v>
       </c>
       <c r="D56">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E56">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="F56">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G56">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H56">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="57" spans="1:8">
@@ -2075,10 +2075,10 @@
         <v>16</v>
       </c>
       <c r="F57">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G57">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H57">
         <v>16</v>
@@ -2115,25 +2115,25 @@
         <v>65</v>
       </c>
       <c r="B59" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C59" t="s">
         <v>74</v>
       </c>
       <c r="D59">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E59">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F59">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G59">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H59">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:8">
@@ -2153,13 +2153,13 @@
         <v>16</v>
       </c>
       <c r="F60">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G60">
         <v>16</v>
       </c>
       <c r="H60">
-        <v>4</v>
+        <v>16</v>
       </c>
     </row>
     <row r="61" spans="1:8">
@@ -2185,7 +2185,7 @@
         <v>16</v>
       </c>
       <c r="H61">
-        <v>16</v>
+        <v>4</v>
       </c>
     </row>
     <row r="62" spans="1:8">
@@ -2219,16 +2219,16 @@
         <v>69</v>
       </c>
       <c r="B63" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C63" t="s">
         <v>74</v>
       </c>
       <c r="D63">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E63">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="F63">
         <v>16</v>

</xml_diff>

<commit_message>
feat: Implement GT-Z Strict D-1 Audit Protocol (Target 8 Decks on Sat)
</commit_message>
<xml_diff>
--- a/data/relatorio_participacao_guerra.xlsx
+++ b/data/relatorio_participacao_guerra.xlsx
@@ -106,124 +106,124 @@
     <t>dogmal</t>
   </si>
   <si>
+    <t>^_^^_^</t>
+  </si>
+  <si>
+    <t>WILLIAN</t>
+  </si>
+  <si>
+    <t>Pedro PH</t>
+  </si>
+  <si>
+    <t>Chetto</t>
+  </si>
+  <si>
+    <t>Alvaro</t>
+  </si>
+  <si>
+    <t>Nico</t>
+  </si>
+  <si>
+    <t>luck</t>
+  </si>
+  <si>
+    <t>polaris</t>
+  </si>
+  <si>
+    <t>GabiMalvadeza</t>
+  </si>
+  <si>
+    <t>tavin</t>
+  </si>
+  <si>
+    <t>Grimmer 狼</t>
+  </si>
+  <si>
+    <t>Rodolfos</t>
+  </si>
+  <si>
+    <t>Bruno</t>
+  </si>
+  <si>
+    <t>super</t>
+  </si>
+  <si>
+    <t>domador de but</t>
+  </si>
+  <si>
+    <t>gabiggoughost</t>
+  </si>
+  <si>
+    <t>Mila</t>
+  </si>
+  <si>
+    <t>Daniele❤</t>
+  </si>
+  <si>
+    <t>WvCly</t>
+  </si>
+  <si>
+    <t>Teixeirazzqw</t>
+  </si>
+  <si>
+    <t>Dockz</t>
+  </si>
+  <si>
+    <t>Luciano</t>
+  </si>
+  <si>
+    <t>gabriel 3$</t>
+  </si>
+  <si>
+    <t>filho de duque</t>
+  </si>
+  <si>
+    <t>ZackThunder</t>
+  </si>
+  <si>
+    <t>joão3:16</t>
+  </si>
+  <si>
+    <t>RobaFrag</t>
+  </si>
+  <si>
+    <t>Sotto ツ</t>
+  </si>
+  <si>
+    <t>OneDePrata</t>
+  </si>
+  <si>
+    <t>mathi❄️</t>
+  </si>
+  <si>
+    <t>Gustavo Clash</t>
+  </si>
+  <si>
     <t>RaiNascimento</t>
   </si>
   <si>
-    <t>^_^^_^</t>
-  </si>
-  <si>
-    <t>Bruno</t>
-  </si>
-  <si>
-    <t>domador de but</t>
-  </si>
-  <si>
-    <t>Nico</t>
-  </si>
-  <si>
-    <t>Pedro PH</t>
-  </si>
-  <si>
-    <t>WILLIAN</t>
-  </si>
-  <si>
-    <t>gabiggoughost</t>
-  </si>
-  <si>
-    <t>polaris</t>
-  </si>
-  <si>
-    <t>Sotto ツ</t>
-  </si>
-  <si>
-    <t>mathi❄️</t>
-  </si>
-  <si>
-    <t>Gustavo Clash</t>
-  </si>
-  <si>
-    <t>Chetto</t>
-  </si>
-  <si>
-    <t>GabiMalvadeza</t>
-  </si>
-  <si>
-    <t>Alvaro</t>
-  </si>
-  <si>
-    <t>Teixeirazzqw</t>
-  </si>
-  <si>
-    <t>Rodolfos</t>
-  </si>
-  <si>
-    <t>filho de duque</t>
-  </si>
-  <si>
-    <t>luck</t>
-  </si>
-  <si>
-    <t>tavin</t>
+    <t>andrebts</t>
+  </si>
+  <si>
+    <t>⭐O SENTINELA ⭐</t>
   </si>
   <si>
     <t>O GUARDIÃO</t>
   </si>
   <si>
-    <t>Grimmer 狼</t>
-  </si>
-  <si>
-    <t>super</t>
+    <t>DGJ-DAVI</t>
+  </si>
+  <si>
+    <t>51 é pinga</t>
   </si>
   <si>
     <t>EDDIE</t>
   </si>
   <si>
-    <t>⭐O SENTINELA ⭐</t>
-  </si>
-  <si>
-    <t>andrebts</t>
-  </si>
-  <si>
-    <t>OneDePrata</t>
-  </si>
-  <si>
-    <t>Dockz</t>
-  </si>
-  <si>
-    <t>Mila</t>
-  </si>
-  <si>
-    <t>RobaFrag</t>
-  </si>
-  <si>
-    <t>Daniele❤</t>
-  </si>
-  <si>
-    <t>51 é pinga</t>
-  </si>
-  <si>
-    <t>WvCly</t>
-  </si>
-  <si>
-    <t>DGJ-DAVI</t>
-  </si>
-  <si>
     <t>isp</t>
   </si>
   <si>
     <t>nivelador</t>
-  </si>
-  <si>
-    <t>Luciano</t>
-  </si>
-  <si>
-    <t>gabriel 3$</t>
-  </si>
-  <si>
-    <t>ZackThunder</t>
-  </si>
-  <si>
-    <t>joão3:16</t>
   </si>
   <si>
     <t>Asten Acady</t>
@@ -1205,25 +1205,25 @@
         <v>30</v>
       </c>
       <c r="B24" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C24" t="s">
         <v>74</v>
       </c>
       <c r="D24">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="E24">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="F24">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="G24">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="H24">
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -1231,25 +1231,25 @@
         <v>31</v>
       </c>
       <c r="B25" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C25" t="s">
         <v>74</v>
       </c>
       <c r="D25">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="E25">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="F25">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="G25">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="H25">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -1269,13 +1269,13 @@
         <v>16</v>
       </c>
       <c r="F26">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G26">
         <v>0</v>
       </c>
       <c r="H26">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -1283,25 +1283,25 @@
         <v>33</v>
       </c>
       <c r="B27" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C27" t="s">
         <v>74</v>
       </c>
       <c r="D27">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E27">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F27">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="G27">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="H27">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -1315,19 +1315,19 @@
         <v>74</v>
       </c>
       <c r="D28">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E28">
         <v>14</v>
       </c>
       <c r="F28">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="G28">
         <v>14</v>
       </c>
       <c r="H28">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -1335,25 +1335,25 @@
         <v>35</v>
       </c>
       <c r="B29" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C29" t="s">
         <v>74</v>
       </c>
       <c r="D29">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E29">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F29">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G29">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="H29">
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -1361,25 +1361,25 @@
         <v>36</v>
       </c>
       <c r="B30" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C30" t="s">
         <v>74</v>
       </c>
       <c r="D30">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E30">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="F30">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="G30">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="H30">
-        <v>0</v>
+        <v>13</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -1396,7 +1396,7 @@
         <v>16</v>
       </c>
       <c r="E31">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F31">
         <v>16</v>
@@ -1413,25 +1413,25 @@
         <v>38</v>
       </c>
       <c r="B32" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C32" t="s">
         <v>74</v>
       </c>
       <c r="D32">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="E32">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="F32">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="G32">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="H32">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -1448,13 +1448,13 @@
         <v>12</v>
       </c>
       <c r="E33">
+        <v>8</v>
+      </c>
+      <c r="F33">
         <v>14</v>
       </c>
-      <c r="F33">
-        <v>12</v>
-      </c>
       <c r="G33">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H33">
         <v>16</v>
@@ -1465,25 +1465,25 @@
         <v>40</v>
       </c>
       <c r="B34" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C34" t="s">
         <v>74</v>
       </c>
       <c r="D34">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E34">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F34">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="G34">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="H34">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -1506,10 +1506,10 @@
         <v>16</v>
       </c>
       <c r="G35">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H35">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -1517,25 +1517,25 @@
         <v>42</v>
       </c>
       <c r="B36" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C36" t="s">
         <v>74</v>
       </c>
       <c r="D36">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E36">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="F36">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="G36">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="H36">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -1543,25 +1543,25 @@
         <v>43</v>
       </c>
       <c r="B37" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C37" t="s">
         <v>74</v>
       </c>
       <c r="D37">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E37">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="F37">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="G37">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="H37">
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="38" spans="1:8">
@@ -1569,25 +1569,25 @@
         <v>44</v>
       </c>
       <c r="B38" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C38" t="s">
         <v>74</v>
       </c>
       <c r="D38">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E38">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F38">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="G38">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H38">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -1595,25 +1595,25 @@
         <v>45</v>
       </c>
       <c r="B39" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C39" t="s">
         <v>74</v>
       </c>
       <c r="D39">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="E39">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="F39">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="G39">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="H39">
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="40" spans="1:8">
@@ -1621,13 +1621,13 @@
         <v>46</v>
       </c>
       <c r="B40" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C40" t="s">
         <v>74</v>
       </c>
       <c r="D40">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E40">
         <v>16</v>
@@ -1636,10 +1636,10 @@
         <v>16</v>
       </c>
       <c r="G40">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H40">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="41" spans="1:8">
@@ -1647,25 +1647,25 @@
         <v>47</v>
       </c>
       <c r="B41" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C41" t="s">
         <v>74</v>
       </c>
       <c r="D41">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E41">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="F41">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="G41">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="H41">
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="42" spans="1:8">
@@ -1673,25 +1673,25 @@
         <v>48</v>
       </c>
       <c r="B42" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C42" t="s">
         <v>74</v>
       </c>
       <c r="D42">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E42">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F42">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="G42">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="H42">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="43" spans="1:8">
@@ -1699,25 +1699,25 @@
         <v>49</v>
       </c>
       <c r="B43" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C43" t="s">
         <v>74</v>
       </c>
       <c r="D43">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E43">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="F43">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="G43">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="H43">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:8">
@@ -1734,7 +1734,7 @@
         <v>16</v>
       </c>
       <c r="E44">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F44">
         <v>16</v>
@@ -1743,7 +1743,7 @@
         <v>16</v>
       </c>
       <c r="H44">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="45" spans="1:8">
@@ -1760,16 +1760,16 @@
         <v>16</v>
       </c>
       <c r="E45">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="F45">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="G45">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="H45">
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="46" spans="1:8">
@@ -1795,7 +1795,7 @@
         <v>16</v>
       </c>
       <c r="H46">
-        <v>16</v>
+        <v>4</v>
       </c>
     </row>
     <row r="47" spans="1:8">
@@ -1803,25 +1803,25 @@
         <v>53</v>
       </c>
       <c r="B47" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C47" t="s">
         <v>74</v>
       </c>
       <c r="D47">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="E47">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="F47">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="G47">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="H47">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:8">
@@ -1838,7 +1838,7 @@
         <v>16</v>
       </c>
       <c r="E48">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="F48">
         <v>16</v>
@@ -1847,7 +1847,7 @@
         <v>16</v>
       </c>
       <c r="H48">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="49" spans="1:8">
@@ -1855,13 +1855,13 @@
         <v>55</v>
       </c>
       <c r="B49" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C49" t="s">
         <v>74</v>
       </c>
       <c r="D49">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E49">
         <v>16</v>
@@ -1881,22 +1881,22 @@
         <v>56</v>
       </c>
       <c r="B50" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C50" t="s">
         <v>74</v>
       </c>
       <c r="D50">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E50">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="F50">
         <v>16</v>
       </c>
       <c r="G50">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H50">
         <v>16</v>
@@ -1907,25 +1907,25 @@
         <v>57</v>
       </c>
       <c r="B51" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C51" t="s">
         <v>74</v>
       </c>
       <c r="D51">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E51">
         <v>14</v>
       </c>
       <c r="F51">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G51">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H51">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="52" spans="1:8">
@@ -1933,22 +1933,22 @@
         <v>58</v>
       </c>
       <c r="B52" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C52" t="s">
         <v>74</v>
       </c>
       <c r="D52">
+        <v>15</v>
+      </c>
+      <c r="E52">
         <v>8</v>
       </c>
-      <c r="E52">
-        <v>16</v>
-      </c>
       <c r="F52">
         <v>16</v>
       </c>
       <c r="G52">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H52">
         <v>16</v>
@@ -1959,16 +1959,16 @@
         <v>59</v>
       </c>
       <c r="B53" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C53" t="s">
         <v>74</v>
       </c>
       <c r="D53">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E53">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F53">
         <v>16</v>
@@ -2011,25 +2011,25 @@
         <v>61</v>
       </c>
       <c r="B55" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C55" t="s">
         <v>74</v>
       </c>
       <c r="D55">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="E55">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="F55">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="G55">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="H55">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:8">
@@ -2037,25 +2037,25 @@
         <v>62</v>
       </c>
       <c r="B56" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C56" t="s">
         <v>74</v>
       </c>
       <c r="D56">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="E56">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F56">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="G56">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="H56">
-        <v>6</v>
+        <v>16</v>
       </c>
     </row>
     <row r="57" spans="1:8">
@@ -2075,10 +2075,10 @@
         <v>16</v>
       </c>
       <c r="F57">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="G57">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H57">
         <v>16</v>
@@ -2115,25 +2115,25 @@
         <v>65</v>
       </c>
       <c r="B59" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C59" t="s">
         <v>74</v>
       </c>
       <c r="D59">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E59">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="F59">
+        <v>12</v>
+      </c>
+      <c r="G59">
         <v>15</v>
       </c>
-      <c r="G59">
-        <v>12</v>
-      </c>
       <c r="H59">
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="60" spans="1:8">
@@ -2153,7 +2153,7 @@
         <v>16</v>
       </c>
       <c r="F60">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G60">
         <v>16</v>
@@ -2185,7 +2185,7 @@
         <v>16</v>
       </c>
       <c r="H61">
-        <v>4</v>
+        <v>16</v>
       </c>
     </row>
     <row r="62" spans="1:8">
@@ -2202,7 +2202,7 @@
         <v>16</v>
       </c>
       <c r="E62">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="F62">
         <v>16</v>
@@ -2211,7 +2211,7 @@
         <v>16</v>
       </c>
       <c r="H62">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="63" spans="1:8">
@@ -2219,25 +2219,25 @@
         <v>69</v>
       </c>
       <c r="B63" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C63" t="s">
         <v>74</v>
       </c>
       <c r="D63">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E63">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F63">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G63">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H63">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:8">

</xml_diff>

<commit_message>
chore(auto): pipeline update & logic validation
</commit_message>
<xml_diff>
--- a/data/relatorio_participacao_guerra.xlsx
+++ b/data/relatorio_participacao_guerra.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="76">
   <si>
     <t>Nome</t>
   </si>
@@ -106,127 +106,130 @@
     <t>dogmal</t>
   </si>
   <si>
+    <t>StelaAby</t>
+  </si>
+  <si>
     <t>^_^^_^</t>
   </si>
   <si>
     <t>WILLIAN</t>
   </si>
   <si>
+    <t>Chetto</t>
+  </si>
+  <si>
+    <t>Alvaro</t>
+  </si>
+  <si>
+    <t>Nico</t>
+  </si>
+  <si>
     <t>Pedro PH</t>
   </si>
   <si>
-    <t>Chetto</t>
-  </si>
-  <si>
-    <t>Alvaro</t>
-  </si>
-  <si>
-    <t>Nico</t>
+    <t>polaris</t>
+  </si>
+  <si>
+    <t>GabiMalvadeza</t>
+  </si>
+  <si>
+    <t>tavin</t>
+  </si>
+  <si>
+    <t>Grimmer 狼</t>
+  </si>
+  <si>
+    <t>Rodolfos</t>
+  </si>
+  <si>
+    <t>super</t>
+  </si>
+  <si>
+    <t>domador de but</t>
+  </si>
+  <si>
+    <t>gabiggoughost</t>
+  </si>
+  <si>
+    <t>Daniele❤</t>
+  </si>
+  <si>
+    <t>Teixeirazzqw</t>
+  </si>
+  <si>
+    <t>Luciano</t>
+  </si>
+  <si>
+    <t>filho de duque</t>
+  </si>
+  <si>
+    <t>Sotto ツ</t>
+  </si>
+  <si>
+    <t>OneDePrata</t>
+  </si>
+  <si>
+    <t>mathi❄️</t>
+  </si>
+  <si>
+    <t>Gustavo Clash</t>
+  </si>
+  <si>
+    <t>Dockz</t>
+  </si>
+  <si>
+    <t>RaiNascimento</t>
   </si>
   <si>
     <t>luck</t>
   </si>
   <si>
-    <t>polaris</t>
-  </si>
-  <si>
-    <t>GabiMalvadeza</t>
-  </si>
-  <si>
-    <t>tavin</t>
-  </si>
-  <si>
-    <t>Grimmer 狼</t>
-  </si>
-  <si>
-    <t>Rodolfos</t>
-  </si>
-  <si>
     <t>Bruno</t>
   </si>
   <si>
-    <t>super</t>
-  </si>
-  <si>
-    <t>domador de but</t>
-  </si>
-  <si>
-    <t>gabiggoughost</t>
+    <t>andrebts</t>
+  </si>
+  <si>
+    <t>⭐O SENTINELA ⭐</t>
+  </si>
+  <si>
+    <t>O GUARDIÃO</t>
+  </si>
+  <si>
+    <t>DGJ-DAVI</t>
+  </si>
+  <si>
+    <t>51 é pinga</t>
+  </si>
+  <si>
+    <t>EDDIE</t>
+  </si>
+  <si>
+    <t>WvCly</t>
+  </si>
+  <si>
+    <t>isp</t>
   </si>
   <si>
     <t>Mila</t>
   </si>
   <si>
-    <t>Daniele❤</t>
-  </si>
-  <si>
-    <t>WvCly</t>
-  </si>
-  <si>
-    <t>Teixeirazzqw</t>
-  </si>
-  <si>
-    <t>Dockz</t>
-  </si>
-  <si>
-    <t>Luciano</t>
-  </si>
-  <si>
     <t>gabriel 3$</t>
   </si>
   <si>
-    <t>filho de duque</t>
+    <t>nivelador</t>
+  </si>
+  <si>
+    <t>Asten Acady</t>
+  </si>
+  <si>
+    <t>joão3:16</t>
   </si>
   <si>
     <t>ZackThunder</t>
   </si>
   <si>
-    <t>joão3:16</t>
-  </si>
-  <si>
     <t>RobaFrag</t>
-  </si>
-  <si>
-    <t>Sotto ツ</t>
-  </si>
-  <si>
-    <t>OneDePrata</t>
-  </si>
-  <si>
-    <t>mathi❄️</t>
-  </si>
-  <si>
-    <t>Gustavo Clash</t>
-  </si>
-  <si>
-    <t>RaiNascimento</t>
-  </si>
-  <si>
-    <t>andrebts</t>
-  </si>
-  <si>
-    <t>⭐O SENTINELA ⭐</t>
-  </si>
-  <si>
-    <t>O GUARDIÃO</t>
-  </si>
-  <si>
-    <t>DGJ-DAVI</t>
-  </si>
-  <si>
-    <t>51 é pinga</t>
-  </si>
-  <si>
-    <t>EDDIE</t>
-  </si>
-  <si>
-    <t>isp</t>
-  </si>
-  <si>
-    <t>nivelador</t>
-  </si>
-  <si>
-    <t>Asten Acady</t>
   </si>
   <si>
     <t>Razoável</t>
@@ -596,7 +599,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H64"/>
+  <dimension ref="A1:H65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -633,10 +636,10 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D2">
         <v>12</v>
@@ -659,10 +662,10 @@
         <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -685,10 +688,10 @@
         <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -711,10 +714,10 @@
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C5" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -737,10 +740,10 @@
         <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C6" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -763,10 +766,10 @@
         <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C7" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -789,10 +792,10 @@
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C8" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -815,10 +818,10 @@
         <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C9" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -841,10 +844,10 @@
         <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C10" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D10">
         <v>3</v>
@@ -867,10 +870,10 @@
         <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C11" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D11">
         <v>16</v>
@@ -893,10 +896,10 @@
         <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C12" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D12">
         <v>14</v>
@@ -919,10 +922,10 @@
         <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C13" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D13">
         <v>0</v>
@@ -945,10 +948,10 @@
         <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C14" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D14">
         <v>0</v>
@@ -971,10 +974,10 @@
         <v>21</v>
       </c>
       <c r="B15" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C15" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D15">
         <v>16</v>
@@ -997,10 +1000,10 @@
         <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C16" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -1023,10 +1026,10 @@
         <v>23</v>
       </c>
       <c r="B17" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C17" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D17">
         <v>9</v>
@@ -1049,10 +1052,10 @@
         <v>24</v>
       </c>
       <c r="B18" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C18" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -1075,10 +1078,10 @@
         <v>25</v>
       </c>
       <c r="B19" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C19" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D19">
         <v>12</v>
@@ -1101,10 +1104,10 @@
         <v>26</v>
       </c>
       <c r="B20" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C20" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D20">
         <v>4</v>
@@ -1127,10 +1130,10 @@
         <v>27</v>
       </c>
       <c r="B21" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C21" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D21">
         <v>0</v>
@@ -1153,10 +1156,10 @@
         <v>28</v>
       </c>
       <c r="B22" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C22" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D22">
         <v>8</v>
@@ -1179,10 +1182,10 @@
         <v>29</v>
       </c>
       <c r="B23" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C23" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D23">
         <v>0</v>
@@ -1205,25 +1208,25 @@
         <v>30</v>
       </c>
       <c r="B24" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C24" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D24">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="E24">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="F24">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="G24">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="H24">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -1234,22 +1237,22 @@
         <v>72</v>
       </c>
       <c r="C25" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D25">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="E25">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="F25">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="G25">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="H25">
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -1260,16 +1263,16 @@
         <v>73</v>
       </c>
       <c r="C26" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D26">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="E26">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="F26">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="G26">
         <v>0</v>
@@ -1283,10 +1286,10 @@
         <v>33</v>
       </c>
       <c r="B27" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C27" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D27">
         <v>12</v>
@@ -1309,10 +1312,10 @@
         <v>34</v>
       </c>
       <c r="B28" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C28" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D28">
         <v>13</v>
@@ -1335,10 +1338,10 @@
         <v>35</v>
       </c>
       <c r="B29" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C29" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D29">
         <v>14</v>
@@ -1361,10 +1364,10 @@
         <v>36</v>
       </c>
       <c r="B30" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C30" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D30">
         <v>16</v>
@@ -1373,13 +1376,13 @@
         <v>16</v>
       </c>
       <c r="F30">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="G30">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="H30">
-        <v>13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -1387,10 +1390,10 @@
         <v>37</v>
       </c>
       <c r="B31" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C31" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D31">
         <v>16</v>
@@ -1413,10 +1416,10 @@
         <v>38</v>
       </c>
       <c r="B32" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C32" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D32">
         <v>0</v>
@@ -1439,10 +1442,10 @@
         <v>39</v>
       </c>
       <c r="B33" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C33" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D33">
         <v>12</v>
@@ -1465,10 +1468,10 @@
         <v>40</v>
       </c>
       <c r="B34" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C34" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D34">
         <v>16</v>
@@ -1491,10 +1494,10 @@
         <v>41</v>
       </c>
       <c r="B35" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C35" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D35">
         <v>16</v>
@@ -1517,10 +1520,10 @@
         <v>42</v>
       </c>
       <c r="B36" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C36" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D36">
         <v>16</v>
@@ -1529,10 +1532,10 @@
         <v>16</v>
       </c>
       <c r="F36">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="G36">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="H36">
         <v>16</v>
@@ -1543,10 +1546,10 @@
         <v>43</v>
       </c>
       <c r="B37" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C37" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D37">
         <v>16</v>
@@ -1555,13 +1558,13 @@
         <v>16</v>
       </c>
       <c r="F37">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="G37">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H37">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="38" spans="1:8">
@@ -1569,25 +1572,25 @@
         <v>44</v>
       </c>
       <c r="B38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C38" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D38">
         <v>16</v>
       </c>
       <c r="E38">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F38">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="G38">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="H38">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -1595,16 +1598,16 @@
         <v>45</v>
       </c>
       <c r="B39" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C39" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D39">
         <v>16</v>
       </c>
       <c r="E39">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F39">
         <v>16</v>
@@ -1621,25 +1624,25 @@
         <v>46</v>
       </c>
       <c r="B40" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C40" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D40">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E40">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="F40">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="G40">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="H40">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:8">
@@ -1647,10 +1650,10 @@
         <v>47</v>
       </c>
       <c r="B41" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C41" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D41">
         <v>16</v>
@@ -1659,7 +1662,7 @@
         <v>16</v>
       </c>
       <c r="F41">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G41">
         <v>16</v>
@@ -1673,25 +1676,25 @@
         <v>48</v>
       </c>
       <c r="B42" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C42" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D42">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="E42">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="F42">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="G42">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="H42">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:8">
@@ -1702,22 +1705,22 @@
         <v>72</v>
       </c>
       <c r="C43" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D43">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E43">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="F43">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="G43">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="H43">
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="44" spans="1:8">
@@ -1725,25 +1728,25 @@
         <v>50</v>
       </c>
       <c r="B44" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C44" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D44">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E44">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="F44">
         <v>16</v>
       </c>
       <c r="G44">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H44">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="45" spans="1:8">
@@ -1751,19 +1754,19 @@
         <v>51</v>
       </c>
       <c r="B45" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C45" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D45">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E45">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F45">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G45">
         <v>16</v>
@@ -1777,10 +1780,10 @@
         <v>52</v>
       </c>
       <c r="B46" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C46" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D46">
         <v>16</v>
@@ -1795,7 +1798,7 @@
         <v>16</v>
       </c>
       <c r="H46">
-        <v>4</v>
+        <v>16</v>
       </c>
     </row>
     <row r="47" spans="1:8">
@@ -1803,25 +1806,25 @@
         <v>53</v>
       </c>
       <c r="B47" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C47" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D47">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E47">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="F47">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="G47">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="H47">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="48" spans="1:8">
@@ -1832,22 +1835,22 @@
         <v>73</v>
       </c>
       <c r="C48" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D48">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="E48">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="F48">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="G48">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="H48">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:8">
@@ -1855,10 +1858,10 @@
         <v>55</v>
       </c>
       <c r="B49" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C49" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D49">
         <v>16</v>
@@ -1867,13 +1870,13 @@
         <v>16</v>
       </c>
       <c r="F49">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G49">
         <v>16</v>
       </c>
       <c r="H49">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="50" spans="1:8">
@@ -1881,10 +1884,10 @@
         <v>56</v>
       </c>
       <c r="B50" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C50" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D50">
         <v>16</v>
@@ -1893,10 +1896,10 @@
         <v>16</v>
       </c>
       <c r="F50">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="G50">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="H50">
         <v>16</v>
@@ -1907,22 +1910,22 @@
         <v>57</v>
       </c>
       <c r="B51" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C51" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D51">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E51">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F51">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="G51">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H51">
         <v>16</v>
@@ -1933,22 +1936,22 @@
         <v>58</v>
       </c>
       <c r="B52" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C52" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D52">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E52">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="F52">
         <v>16</v>
       </c>
       <c r="G52">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H52">
         <v>16</v>
@@ -1959,16 +1962,16 @@
         <v>59</v>
       </c>
       <c r="B53" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C53" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D53">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E53">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="F53">
         <v>16</v>
@@ -1985,10 +1988,10 @@
         <v>60</v>
       </c>
       <c r="B54" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C54" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D54">
         <v>16</v>
@@ -1997,10 +2000,10 @@
         <v>16</v>
       </c>
       <c r="F54">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G54">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H54">
         <v>16</v>
@@ -2011,25 +2014,25 @@
         <v>61</v>
       </c>
       <c r="B55" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C55" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D55">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E55">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="F55">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="G55">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="H55">
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="56" spans="1:8">
@@ -2037,13 +2040,13 @@
         <v>62</v>
       </c>
       <c r="B56" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C56" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D56">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E56">
         <v>16</v>
@@ -2066,22 +2069,22 @@
         <v>73</v>
       </c>
       <c r="C57" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D57">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E57">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F57">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="G57">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="H57">
-        <v>16</v>
+        <v>6</v>
       </c>
     </row>
     <row r="58" spans="1:8">
@@ -2089,10 +2092,10 @@
         <v>64</v>
       </c>
       <c r="B58" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C58" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D58">
         <v>16</v>
@@ -2118,19 +2121,19 @@
         <v>73</v>
       </c>
       <c r="C59" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D59">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E59">
         <v>16</v>
       </c>
       <c r="F59">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="G59">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H59">
         <v>16</v>
@@ -2141,10 +2144,10 @@
         <v>66</v>
       </c>
       <c r="B60" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C60" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D60">
         <v>16</v>
@@ -2159,7 +2162,7 @@
         <v>16</v>
       </c>
       <c r="H60">
-        <v>16</v>
+        <v>4</v>
       </c>
     </row>
     <row r="61" spans="1:8">
@@ -2167,25 +2170,25 @@
         <v>67</v>
       </c>
       <c r="B61" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C61" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D61">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E61">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F61">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G61">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H61">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:8">
@@ -2193,10 +2196,10 @@
         <v>68</v>
       </c>
       <c r="B62" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C62" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D62">
         <v>16</v>
@@ -2219,25 +2222,25 @@
         <v>69</v>
       </c>
       <c r="B63" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C63" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D63">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E63">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="F63">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G63">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="H63">
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="64" spans="1:8">
@@ -2245,16 +2248,16 @@
         <v>70</v>
       </c>
       <c r="B64" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C64" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D64">
         <v>16</v>
       </c>
       <c r="E64">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="F64">
         <v>16</v>
@@ -2263,6 +2266,32 @@
         <v>16</v>
       </c>
       <c r="H64">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8">
+      <c r="A65" t="s">
+        <v>71</v>
+      </c>
+      <c r="B65" t="s">
+        <v>74</v>
+      </c>
+      <c r="C65" t="s">
+        <v>75</v>
+      </c>
+      <c r="D65">
+        <v>16</v>
+      </c>
+      <c r="E65">
+        <v>16</v>
+      </c>
+      <c r="F65">
+        <v>16</v>
+      </c>
+      <c r="G65">
+        <v>16</v>
+      </c>
+      <c r="H65">
         <v>16</v>
       </c>
     </row>

</xml_diff>